<commit_message>
auto commit @21.01.2021: 19:26:02,26
</commit_message>
<xml_diff>
--- a/FACT Analyse/analysis.xlsx
+++ b/FACT Analyse/analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Benutzer\Henry\Downloads\Abschlussarbeit_H-BRS\FACT Analyse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Benutzer\Henry\Downloads\Thesis\Abschlussarbeit_H-BRS\FACT Analyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7E7C24-AD57-4C49-828D-E1C6FEF486D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99632A1D-57D9-4D45-A51D-3EE4B03096C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -38,27 +38,27 @@
     <definedName name="_xlchart.v1.19" hidden="1">'Exploit Mitigations'!$Z$93</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">CVEs!$A$12:$A$18</definedName>
     <definedName name="_xlchart.v1.20" hidden="1">'Exploit Mitigations'!$Z$94:$Z$100</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">'Exploit Mitigations'!$X$46:$X$52</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">'Exploit Mitigations'!$Y$45</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">'Exploit Mitigations'!$Y$46:$Y$52</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">'Exploit Mitigations'!$X$61:$X$67</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">'Exploit Mitigations'!$Y$60</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">'Exploit Mitigations'!$Y$61:$Y$67</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">'Exploit Mitigations'!$X$77:$X$83</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">'Exploit Mitigations'!$Y$76</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">'Exploit Mitigations'!$Y$77:$Y$83</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">'Exploit Mitigations'!$X$61:$X$67</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">'Exploit Mitigations'!$Y$60</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">'Exploit Mitigations'!$Y$61:$Y$67</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">'Exploit Mitigations'!$X$15:$X$21</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">'Exploit Mitigations'!$Y$14</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">'Exploit Mitigations'!$Y$15:$Y$21</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">'Exploit Mitigations'!$X$28:$X$34</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">'Exploit Mitigations'!$Y$27</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">'Exploit Mitigations'!$Y$28:$Y$34</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">CVEs!$B$12:$B$18</definedName>
     <definedName name="_xlchart.v1.30" hidden="1">'Private Keys'!$A$11:$A$17</definedName>
     <definedName name="_xlchart.v1.31" hidden="1">'Private Keys'!$B$11:$B$17</definedName>
     <definedName name="_xlchart.v1.32" hidden="1">'Login Credentials'!$A$20:$A$26</definedName>
     <definedName name="_xlchart.v1.33" hidden="1">'Login Credentials'!$B$19</definedName>
     <definedName name="_xlchart.v1.34" hidden="1">'Login Credentials'!$B$20:$B$26</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Exploit Mitigations'!$X$15:$X$21</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Exploit Mitigations'!$Y$14</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Exploit Mitigations'!$Y$15:$Y$21</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Exploit Mitigations'!$X$28:$X$34</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'Exploit Mitigations'!$Y$27</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'Exploit Mitigations'!$Y$28:$Y$34</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'Exploit Mitigations'!$X$46:$X$52</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'Exploit Mitigations'!$Y$45</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'Exploit Mitigations'!$Y$46:$Y$52</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'Exploit Mitigations'!$X$77:$X$83</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'Exploit Mitigations'!$Y$76</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'Exploit Mitigations'!$Y$77:$Y$83</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -673,62 +673,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="de-DE"/>
-              <a:t>Tage seit dem letzten Update pro Firmware-Abbild</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -774,7 +719,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -1154,7 +1099,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1213,7 +1158,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1255,7 +1200,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2508,67 +2453,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="de-DE"/>
-              <a:t>Number of Private</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="de-DE" baseline="0"/>
-              <a:t> Keys per Firmware Image</a:t>
-            </a:r>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -2905,7 +2790,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2931,7 +2816,7 @@
         <c:axId val="334163487"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="12"/>
+          <c:max val="2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2965,7 +2850,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2983,6 +2868,7 @@
         <c:crossAx val="336027551"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="1"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -5069,95 +4955,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:buClrTx/>
-              <a:buSzTx/>
-              <a:buFontTx/>
-              <a:buNone/>
-              <a:tabLst/>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="de-DE" sz="1600" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Mean of Enabled Exploit Mitigations for all firmwares</a:t>
-            </a:r>
-            <a:endParaRPr lang="de-DE" sz="1600">
-              <a:effectLst/>
-            </a:endParaRPr>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:sysClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:radarChart>
@@ -5272,7 +5070,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -5331,7 +5129,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -5416,62 +5214,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="de-DE"/>
-              <a:t>Percentage of Executables with Exploit Mitigations Enabled per Firmware Image</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -5965,7 +5708,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -6025,7 +5768,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -6067,7 +5810,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -8091,10 +7834,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.24</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.26</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -8132,7 +7875,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{74781C89-E927-480E-80DD-826A021A7BE6}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.5</cx:f>
+              <cx:f>_xlchart.v1.25</cx:f>
               <cx:v>Canary</cx:v>
             </cx:txData>
           </cx:tx>
@@ -8162,10 +7905,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.27</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.29</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -8203,7 +7946,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{CD3D3AFB-F0EC-4041-B623-F269D1568799}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.8</cx:f>
+              <cx:f>_xlchart.v1.28</cx:f>
               <cx:v>FORTIFY_SOURCE</cx:v>
             </cx:txData>
           </cx:tx>
@@ -8233,10 +7976,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.21</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.23</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -8279,7 +8022,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{1CA3B0AF-FBE2-488E-B37A-23AFB12F8190}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.22</cx:f>
+              <cx:f>_xlchart.v1.5</cx:f>
               <cx:v>NX</cx:v>
             </cx:txData>
           </cx:tx>
@@ -8309,10 +8052,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.24</cx:f>
+        <cx:f>_xlchart.v1.21</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.26</cx:f>
+        <cx:f>_xlchart.v1.23</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -8350,7 +8093,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{CB34B628-E6B1-446E-B79D-F3313E9206C4}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.25</cx:f>
+              <cx:f>_xlchart.v1.22</cx:f>
               <cx:v>PIE</cx:v>
             </cx:txData>
           </cx:tx>
@@ -8380,10 +8123,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.27</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.29</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -8438,7 +8181,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{806C733D-0DB2-4503-BAB8-C8F2E4F8C162}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.28</cx:f>
+              <cx:f>_xlchart.v1.8</cx:f>
               <cx:v>RELRO</cx:v>
             </cx:txData>
           </cx:tx>
@@ -21717,8 +21460,8 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>97</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -23548,7 +23291,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FC8CDAC-A32A-463D-B45B-72E9FA4461F8}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -23794,7 +23537,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -24381,8 +24124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AC100"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P74" sqref="P74"/>
+    <sheetView topLeftCell="G74" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G84" sqref="G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -26391,7 +26134,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -26580,7 +26323,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3739379-3DDD-44F6-A7F6-C36B7F0CAD1C}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>

</xml_diff>